<commit_message>
Installation Google search control
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DEAC3D7-8AAF-4F74-848F-A042360960BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B8E5E-D5F9-4AE5-8E0B-22895637E181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6945" yWindow="195" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Categorie</t>
   </si>
@@ -41,6 +41,42 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>JS non minifier</t>
+  </si>
+  <si>
+    <t>meta description &amp; title</t>
+  </si>
+  <si>
+    <t>meta keywords ?</t>
+  </si>
+  <si>
+    <t>balise title ??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!! Black Hat mot nav bar : class keywords </t>
+  </si>
+  <si>
+    <t>liens 404 errors</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>seo</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>langue balise</t>
+  </si>
+  <si>
+    <t>analyse rapide index.html</t>
+  </si>
+  <si>
+    <t>revoir le responsive</t>
   </si>
 </sst>
 </file>
@@ -328,7 +364,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -386,14 +422,69 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Annexe et modification début
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B8E5E-D5F9-4AE5-8E0B-22895637E181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A040ACC-38D1-4033-92BD-515095A5BBC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6945" yWindow="195" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
   <si>
     <t>Categorie</t>
   </si>
@@ -37,53 +37,417 @@
     <t>Action recommandée</t>
   </si>
   <si>
-    <t>Référence</t>
-  </si>
-  <si>
     <t>(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t>JS non minifier</t>
-  </si>
-  <si>
-    <t>meta description &amp; title</t>
-  </si>
-  <si>
-    <t>meta keywords ?</t>
-  </si>
-  <si>
-    <t>balise title ??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!!! Black Hat mot nav bar : class keywords </t>
-  </si>
-  <si>
     <t>liens 404 errors</t>
   </si>
   <si>
     <t>??</t>
   </si>
   <si>
-    <t>seo</t>
-  </si>
-  <si>
-    <t>access</t>
-  </si>
-  <si>
-    <t>langue balise</t>
-  </si>
-  <si>
-    <t>analyse rapide index.html</t>
-  </si>
-  <si>
-    <t>revoir le responsive</t>
+    <t>ERREUR</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Alt identiques</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>description aucune</t>
+  </si>
+  <si>
+    <t>keyword incohérent par rapport au lieux de l'agence lyon / paris</t>
+  </si>
+  <si>
+    <t>contraste</t>
+  </si>
+  <si>
+    <t>nav bar / .keyword</t>
+  </si>
+  <si>
+    <t>présence css dans le fichier html</t>
+  </si>
+  <si>
+    <t>détecté francais paramétré allemand &amp; problème de paramétrage / code &amp; langue par défaut</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Structure HTML H1/H3</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>VITESSE</t>
+  </si>
+  <si>
+    <t>vitesse</t>
+  </si>
+  <si>
+    <t>formats / taille / optimiser</t>
+  </si>
+  <si>
+    <t>différé le chargement js des JS secondaires &amp; minimiser le JS</t>
+  </si>
+  <si>
+    <t>mise en place de cache (24 ressources)</t>
+  </si>
+  <si>
+    <t>PERFORMANCE</t>
+  </si>
+  <si>
+    <t>vérifier css &amp; js non utilisé ?</t>
+  </si>
+  <si>
+    <t>vérifier texte visible et polices d'écriture</t>
+  </si>
+  <si>
+    <t>ACCESSIBILITE</t>
+  </si>
+  <si>
+    <t>Langue non valide</t>
+  </si>
+  <si>
+    <t>Images &amp; créa alt lecteur d'écran</t>
+  </si>
+  <si>
+    <t>MEILLEURES PRATIQUES</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>black hat / texte keyword""</t>
+  </si>
+  <si>
+    <t>liens</t>
+  </si>
+  <si>
+    <t>cible espace autour des liens</t>
+  </si>
+  <si>
+    <t>Images : 93,89% du poids total
+Polices de caractères : 3,34% du poids total
+JavaScript : 1,79% du poids total
+CSS : 0,89% du poids total
+Textes : 0,09% du poids total</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Cette page charge 4.0 Mo de données, diminuez ce poids</t>
+  </si>
+  <si>
+    <t>Selon HTTPArchive, en juillet 2019, le poids moyen d'une page web était de 1,95Mo.</t>
+  </si>
+  <si>
+    <t>6 images (1.0 Mo) sont chargées trop tôt</t>
+  </si>
+  <si>
+    <t>La langue doit être défini en respectant les normes déclaratives</t>
+  </si>
+  <si>
+    <t>(!) BLACK HAT</t>
+  </si>
+  <si>
+    <t>Supprimer ce morceau de code et se concentrer sur les bonnes pratique White Hat pour obtenir un SEO viable et plus stable.</t>
+  </si>
+  <si>
+    <t>SEO &amp; Accessibilité</t>
+  </si>
+  <si>
+    <t>Language du contenu</t>
+  </si>
+  <si>
+    <t>Ne jamais écrire du texte caché aux yeux de l'utilisateur pour essayer de tromper les Bots et gagner en performance SEO.</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Texte en image et taille de police</t>
+  </si>
+  <si>
+    <t>Structure HTML / CSS</t>
+  </si>
+  <si>
+    <t>Vitesse et chargement des ressources</t>
+  </si>
+  <si>
+    <t>Meta données et mots clés</t>
+  </si>
+  <si>
+    <t>Tous les fichiers en lien dans la page doivent être utilisé.</t>
+  </si>
+  <si>
+    <t>Les bots sont des vrais marathoniens ! 
+Pensons donc à ne pas surcharger leur parcours avec des fichiers qui ne sont pas utilisés ni utile au fonctionnement du site.</t>
+  </si>
+  <si>
+    <t>Les images doit être dimensionnées raisonnablement par rapport à son "encart d'accueil", optimisées et être dans un format adapté au web. Elles doivent comportées une description dans un champs 'alt' personnalisé pour les lecteurs d'écran et une largeur appliquée.</t>
+  </si>
+  <si>
+    <t>Sécurité ??</t>
+  </si>
+  <si>
+    <t>Bien renseigné la meta description et ne plus utiliser la meta keywords avec du contenu cohérent au sujet du site. Les mots clés doivent être utilisés de manière intelligente et non répétés sans contexte. Cela s'apparentrait à du Black Hat.</t>
+  </si>
+  <si>
+    <t>//éviter les reflux "" // favicon inclus</t>
+  </si>
+  <si>
+    <t>Utilisation des caches navigateurs, différé le chargement des fichiers secondaires et minifier le JS/CSS.
+Attention aussi : 
+- aux ressources chargées trop tôt;
+- aux redondances d'un même code au sein d'une classe.</t>
+  </si>
+  <si>
+    <t>Ressources non chargées</t>
+  </si>
+  <si>
+    <t>Dans le cas où les scripts ne chargeraient pas, il est fortement conseillé d'afficher un message pour l'utilisateur avec la balise noscript</t>
+  </si>
+  <si>
+    <t>Réseaux sociaux</t>
+  </si>
+  <si>
+    <t>Afin d'aider les réseaux sociaux à comprendre votre site, nous conseillons d'intégrer un Open Graph. Open graph sont des meta données qui va aidé les sites comme Facebook a avoir une meilleure compréhension du site.</t>
+  </si>
+  <si>
+    <t>Fichier robot.txt</t>
+  </si>
+  <si>
+    <t>Un fichier robot.txt est à destination des bots. Il est là pour aider nos bots à travailler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le texte doit être visible et donc être paramétré avec une taille minimale surtout lorsqu'il s'agit de données importantes. Un texte ne doit pas être intégré sous forme d'image mais bien insérer en code en tant que texte dans un paragraphe ou une div. Il faut également veillé à sa visibilité par rapport aux éléments qu'il l'entoure. </t>
+  </si>
+  <si>
+    <t>Couleurs et Contrastes : le Ying et le Yang de l'accessibilité de base.</t>
+  </si>
+  <si>
+    <t>Ci-dessous mon brouillon</t>
+  </si>
+  <si>
+    <r>
+      <t>Panda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : lancé en février 2011, cet algorithme sert à pénaliser les sites ayant du contenu de mauvaise qualité (pas assez de contenu, trop de spam, etc). Mis à jour régulièrement, cet algorithme a été totalement intégré au cœur de Google courant 2015.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pingouin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : cet algorithme lutte contre la création intempestive de liens. Il a été créé en avril 2012, puis intégré au cœur de Google en 2016. Avant la création de cet algorithme, il était très simple de créer des milliers de liens pour se retrouver en première page de Google.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hummingbird/Colibri et son amélioration, Rankbrain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : introduits respectivement en septembre 2013 et début 2015, ce sont ces algorithmes qui permettent à Google de comprendre le contexte d'un mot ou d'une phrase, ou même de comprendre lorsque vous posez une question pour vous donner directement la réponse.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pigeon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: déployé en juin 2015, il favorise les résultats de recherche locaux et l'affichage sur Google Maps.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/webmastering/site-rapide</t>
+  </si>
+  <si>
+    <t>Backlinks</t>
+  </si>
+  <si>
+    <t>Algorithme Google Pingouin (2012)
+https://www.webrankinfo.com/dossiers/google-search/penguin
+https://www.webrankinfo.com/dossiers/gwt/refuser-backlinks
+https://www.webrankinfo.com/dossiers/strategies-de-liens/techniques-netlinking
+https://www.webrankinfo.com/dossiers/strategies-de-liens/backlinks-sitewide</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QWL864VlW7I
+John Mueller (webmaster trends analyst chez Google) dans un hangout avec les webmasters le 11/09/2015
+https://www.webrankinfo.com/dossiers/techniques/balises-h1-h2-h3</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/techniques/idees-seo</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/referencement-mobile/speed-update
+https://www.webrankinfo.com/dossiers/webmastering/site-rapide</t>
+  </si>
+  <si>
+    <t>Cours OC Augmentez votre trafic grâce au référencement naturel</t>
+  </si>
+  <si>
+    <t>Les mots-clés ne sont pas cohérents avec le positionnement de l'agence (ex : Lyon/paris). Il faut les revoir pour assurer une longue traine efficace.
+La Title et la Meta Description sont les deux facteurs qui vont influencer grandement le choix d’un utilisateur entre les différents résultats proposés par les moteurs de recherche. La meta keyword n'est pas essentiel mais Google utilise la meta desciption et la title. Dans notre cas, ni l'une ni l'autre n'est exploitée et correctement utilisée.</t>
+  </si>
+  <si>
+    <t>Utilisation sémantique des balises HTML5 (header, footer, …), construction du code en respectant une hiérarchie logique (h1 -&gt; h2 -&gt; h3 etc) et bien renseigner le title de la page. 
+N'avoir aucun code de style dans le fichier HTML.
+Il faut veiller à ne pas avoir des balises vident afin de ne pas perdre les lecteurs d'écran.</t>
+  </si>
+  <si>
+    <t>htaccesss</t>
+  </si>
+  <si>
+    <t>Revoir la structure HTML5 et la hiérarchie du contenu et enlever les balises ne contenant aucune information.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Structure HTML5 : il faut toujours avoir un header et un footer car</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Nous voyons sur l'index.html que les balises Hn de respectent pas la hiérarchie. Il est important d'utiliser ces balises pour fournir une information sémantique et non l'utiliser pour leur 'visuel'. C'est également un bon moyen d'introduire des mots-clés (expressions). Pour H1, il faut respecter l'ordre de grandeur (80 caractères max). Le H1 doit être légèrement différent de la balise title pour la longue traine.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Le fait d'avoir une structure HTML5 correcte va permettre une meilleure lecture par les bots mais aussi pour les lecteurs d'écran.
+Des balises vides ont un aspect négatif sur les lecteurs d'écran. </t>
+    </r>
+  </si>
+  <si>
+    <t>ARIA ???</t>
+  </si>
+  <si>
+    <t>Références</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/referencement/tout-ce-que-vous-devez-savoir-sur-lopen-graph/
+https://www.referenseo.com/guide-seo/open-graph/
+https://smartkeyword.io/seo-on-page-open-graph-twitter-card/</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>https://www.abondance.com/20200228-42120-infographie-6-points-essentiels-pour-reussir-son-seo-local.html</t>
+  </si>
+  <si>
+    <t>Bichonner sa présence web en définissant un plan Google Business puis de répertorier et gérer les avis de clients pour avoir un meilleur taux de conversion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur la Page 2, le profil de l'entreprise (contact, adresse, horaires, …) n'est pas clairement visible et défini en plus du problème de mots-clés vu juste ci-dessus. Cela frêne le SEO local. 
+</t>
+  </si>
+  <si>
+    <t>Réaliser une véritable campagne de netlinking.
+C'est-à-dire avoir des liens cohérents avec le contenu. Qu'il s'intègre dans l'information pour avoir une vrai plus-value et non une présence superficielle. 
+Liens : titre cohérent, follow les liens cohérents et nofollow les autres (voir les enlever), attribut des liens correctement déclarés.</t>
+  </si>
+  <si>
+    <t>Il faut donc garder ceux qui sont cohérents (et oui soignez vos sources !) et si possible ajouter du contexte/du sens. Envisagez de les enlever carrément du footer et de créer un article/du contenu de qualité en les intégrant pour obtenir du sens et une attraction pour l'utilisateur (situation du lien),
+Mettre des titres cohérents aux liens garder (anchor text)
+Définir si les bots doivent "lire/suivre/regarder" les liens.
+Nous oublions pas de bien déclarer correctement des attribut aux liens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les liens en bas de page (dans le footer visuel) ne sont pas cohérents avec l'activité de l'agence et sont clairement des liens artificiels. On ne comprend pas pourquoi ils sont là. Et n'oublions pas que Google a fait et fait évoluer ses algorithmes pour comprendre le contexte. Des liens "parasites" peuvent faire pénaliser tout le site.  </t>
+  </si>
+  <si>
+    <t>https://analytics.moz.com/pro/keyword-explorer/
+https://support.google.com/webmasters/answer/79812?hl=fr
+Algorithme Google :Colibri et son amélioration, Rankbrain
+https://www.webrankinfo.com/dossiers/conseils/meta-description-seo
+https://www.webrankinfo.com/dossiers/debutants/balise-title
+https://www.webrankinfo.com/dossiers/conseils/balise-meta-description
+https://youtu.be/jK7IPbnmvVU
+https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>Etude sur les mots-clés utilisés et la concurrence.
+Renseigner la balise Title et la Meta description en tilisant les bons mots-clés. Attention, il faut penser utilisateur et compréhension utilisateur ! En effet Google parfait ses algorithmes dans ce sens !
+Enlever la meta keyword qui n'a aucune plus-value car JAMAIS utilisé par les GoggleBots</t>
+  </si>
+  <si>
+    <t>Algorithme Pigeon de Google (2015)
+Cours OC Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques</t>
+  </si>
+  <si>
+    <t>Réaliser une mise en page et</t>
+  </si>
+  <si>
+    <t>Réaliser une multiplication des mots-clés de manière intempestives et cacher à l'utilisateur, que nous pouvons retrouver dans la page index.html et page2.html, est un procédé banni par Google et va même jusqu'à sanctionner en black-listant le site. 
+Index : class=keyword
+Page2 : h1 non visible</t>
+  </si>
+  <si>
+    <t>La langue définie est l'allemand pour un site entièrement écrit en français et les outils d'analyse détectent bien le français.
+Dans la page2, les messages informationnels concernant l'envoi/ou non doivent être dans la même langue.</t>
+  </si>
+  <si>
+    <t>Redéfinir correctement l'attribut lang et ne pas le mettre par défaut ("fr-fr").
+Ecrire en français pour votre auditoire lisant et écoutant (lecteurs d'écran) français.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,8 +469,71 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="2" tint="-4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +544,48 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -136,18 +605,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,20 +908,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
-    <col min="5" max="5" width="43.77734375" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="3" max="5" width="45.5546875" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -394,8 +940,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="F1" s="30" t="s">
+        <v>87</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -418,128 +964,788 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+    </row>
+    <row r="3" spans="1:26" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+    </row>
+    <row r="4" spans="1:26" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+    </row>
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+    </row>
+    <row r="8" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+    </row>
+    <row r="9" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+    </row>
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+    </row>
+    <row r="11" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+    </row>
+    <row r="12" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+    </row>
+    <row r="13" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+    </row>
+    <row r="14" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+    </row>
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+    </row>
+    <row r="16" spans="1:26" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="15"/>
+      <c r="D33" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1476,8 +2682,31 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F18:G23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C49" r:id="rId1" xr:uid="{AB5B6FFC-1D25-4AAE-B717-307BDF0802B7}"/>
+    <hyperlink ref="C50" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fichier d'analyse ok + visu mobile présentation
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A040ACC-38D1-4033-92BD-515095A5BBC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F7A8AE-38C5-449A-9C1F-2E36A13304B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="128">
   <si>
     <t>Categorie</t>
   </si>
@@ -155,15 +155,9 @@
     <t>6 images (1.0 Mo) sont chargées trop tôt</t>
   </si>
   <si>
-    <t>La langue doit être défini en respectant les normes déclaratives</t>
-  </si>
-  <si>
     <t>(!) BLACK HAT</t>
   </si>
   <si>
-    <t>Supprimer ce morceau de code et se concentrer sur les bonnes pratique White Hat pour obtenir un SEO viable et plus stable.</t>
-  </si>
-  <si>
     <t>SEO &amp; Accessibilité</t>
   </si>
   <si>
@@ -191,40 +185,18 @@
     <t>Tous les fichiers en lien dans la page doivent être utilisé.</t>
   </si>
   <si>
-    <t>Les bots sont des vrais marathoniens ! 
-Pensons donc à ne pas surcharger leur parcours avec des fichiers qui ne sont pas utilisés ni utile au fonctionnement du site.</t>
-  </si>
-  <si>
-    <t>Les images doit être dimensionnées raisonnablement par rapport à son "encart d'accueil", optimisées et être dans un format adapté au web. Elles doivent comportées une description dans un champs 'alt' personnalisé pour les lecteurs d'écran et une largeur appliquée.</t>
-  </si>
-  <si>
     <t>Sécurité ??</t>
   </si>
   <si>
     <t>Bien renseigné la meta description et ne plus utiliser la meta keywords avec du contenu cohérent au sujet du site. Les mots clés doivent être utilisés de manière intelligente et non répétés sans contexte. Cela s'apparentrait à du Black Hat.</t>
   </si>
   <si>
-    <t>//éviter les reflux "" // favicon inclus</t>
-  </si>
-  <si>
-    <t>Utilisation des caches navigateurs, différé le chargement des fichiers secondaires et minifier le JS/CSS.
-Attention aussi : 
-- aux ressources chargées trop tôt;
-- aux redondances d'un même code au sein d'une classe.</t>
-  </si>
-  <si>
     <t>Ressources non chargées</t>
   </si>
   <si>
-    <t>Dans le cas où les scripts ne chargeraient pas, il est fortement conseillé d'afficher un message pour l'utilisateur avec la balise noscript</t>
-  </si>
-  <si>
     <t>Réseaux sociaux</t>
   </si>
   <si>
-    <t>Afin d'aider les réseaux sociaux à comprendre votre site, nous conseillons d'intégrer un Open Graph. Open graph sont des meta données qui va aidé les sites comme Facebook a avoir une meilleure compréhension du site.</t>
-  </si>
-  <si>
     <t>Fichier robot.txt</t>
   </si>
   <si>
@@ -232,9 +204,6 @@
   </si>
   <si>
     <t xml:space="preserve">Le texte doit être visible et donc être paramétré avec une taille minimale surtout lorsqu'il s'agit de données importantes. Un texte ne doit pas être intégré sous forme d'image mais bien insérer en code en tant que texte dans un paragraphe ou une div. Il faut également veillé à sa visibilité par rapport aux éléments qu'il l'entoure. </t>
-  </si>
-  <si>
-    <t>Couleurs et Contrastes : le Ying et le Yang de l'accessibilité de base.</t>
   </si>
   <si>
     <t>Ci-dessous mon brouillon</t>
@@ -309,16 +278,7 @@
 https://www.webrankinfo.com/dossiers/strategies-de-liens/backlinks-sitewide</t>
   </si>
   <si>
-    <t>https://youtu.be/QWL864VlW7I
-John Mueller (webmaster trends analyst chez Google) dans un hangout avec les webmasters le 11/09/2015
-https://www.webrankinfo.com/dossiers/techniques/balises-h1-h2-h3</t>
-  </si>
-  <si>
     <t>https://www.webrankinfo.com/dossiers/techniques/idees-seo</t>
-  </si>
-  <si>
-    <t>https://www.webrankinfo.com/dossiers/referencement-mobile/speed-update
-https://www.webrankinfo.com/dossiers/webmastering/site-rapide</t>
   </si>
   <si>
     <t>Cours OC Augmentez votre trafic grâce au référencement naturel</t>
@@ -328,25 +288,130 @@
 La Title et la Meta Description sont les deux facteurs qui vont influencer grandement le choix d’un utilisateur entre les différents résultats proposés par les moteurs de recherche. La meta keyword n'est pas essentiel mais Google utilise la meta desciption et la title. Dans notre cas, ni l'une ni l'autre n'est exploitée et correctement utilisée.</t>
   </si>
   <si>
-    <t>Utilisation sémantique des balises HTML5 (header, footer, …), construction du code en respectant une hiérarchie logique (h1 -&gt; h2 -&gt; h3 etc) et bien renseigner le title de la page. 
-N'avoir aucun code de style dans le fichier HTML.
-Il faut veiller à ne pas avoir des balises vident afin de ne pas perdre les lecteurs d'écran.</t>
-  </si>
-  <si>
-    <t>htaccesss</t>
-  </si>
-  <si>
     <t>Revoir la structure HTML5 et la hiérarchie du contenu et enlever les balises ne contenant aucune information.</t>
   </si>
   <si>
+    <t>ARIA ???</t>
+  </si>
+  <si>
+    <t>Références</t>
+  </si>
+  <si>
+    <t>https://fr.oncrawl.com/referencement/tout-ce-que-vous-devez-savoir-sur-lopen-graph/
+https://www.referenseo.com/guide-seo/open-graph/
+https://smartkeyword.io/seo-on-page-open-graph-twitter-card/</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Réaliser une véritable campagne de netlinking.
+C'est-à-dire avoir des liens cohérents avec le contenu. Qu'il s'intègre dans l'information pour avoir une vrai plus-value et non une présence superficielle. 
+Liens : titre cohérent, follow les liens cohérents et nofollow les autres (voir les enlever), attribut des liens correctement déclarés.</t>
+  </si>
+  <si>
+    <t>Il faut donc garder ceux qui sont cohérents (et oui soignez vos sources !) et si possible ajouter du contexte/du sens. Envisagez de les enlever carrément du footer et de créer un article/du contenu de qualité en les intégrant pour obtenir du sens et une attraction pour l'utilisateur (situation du lien),
+Mettre des titres cohérents aux liens garder (anchor text)
+Définir si les bots doivent "lire/suivre/regarder" les liens.
+Nous oublions pas de bien déclarer correctement des attribut aux liens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les liens en bas de page (dans le footer visuel) ne sont pas cohérents avec l'activité de l'agence et sont clairement des liens artificiels. On ne comprend pas pourquoi ils sont là. Et n'oublions pas que Google a fait et fait évoluer ses algorithmes pour comprendre le contexte. Des liens "parasites" peuvent faire pénaliser tout le site.  </t>
+  </si>
+  <si>
+    <t>https://analytics.moz.com/pro/keyword-explorer/
+https://support.google.com/webmasters/answer/79812?hl=fr
+Algorithme Google :Colibri et son amélioration, Rankbrain
+https://www.webrankinfo.com/dossiers/conseils/meta-description-seo
+https://www.webrankinfo.com/dossiers/debutants/balise-title
+https://www.webrankinfo.com/dossiers/conseils/balise-meta-description
+https://youtu.be/jK7IPbnmvVU
+https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>Etude sur les mots-clés utilisés et la concurrence.
+Renseigner la balise Title et la Meta description en tilisant les bons mots-clés. Attention, il faut penser utilisateur et compréhension utilisateur ! En effet Google parfait ses algorithmes dans ce sens !
+Enlever la meta keyword qui n'a aucune plus-value car JAMAIS utilisé par les GoggleBots</t>
+  </si>
+  <si>
+    <t>La langue définie est l'allemand pour un site entièrement écrit en français et les outils d'analyse détectent bien le français.
+Dans la page2, les messages informationnels concernant l'envoi/ou non doivent être dans la même langue.</t>
+  </si>
+  <si>
+    <t>Redéfinir correctement l'attribut lang et ne pas le mettre par défaut ("fr-fr").
+Ecrire en français pour votre auditoire lisant et écoutant (lecteurs d'écran) français.</t>
+  </si>
+  <si>
+    <t>Supprimer ce morceau de code et se concentrer sur les bonnes pratique White Hat pour obtenir un SEO viable et plus stable. Vous éviterez ainsi de vous faire blacklister par les Googlebots,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Réaliser une multiplication des mots-clés de manière intempestives et cacher à l'utilisateur, que nous pouvons retrouver dans la page index.html et page2.html, est un procédé banni par Google et va même jusqu'à sanctionner en black-listant le site. 
+Index : class=keyword
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFC00000"/>
+        <color theme="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Structure HTML5 : il faut toujours avoir un header et un footer car</t>
+      <t>Page2 : h1 non visible</t>
+    </r>
+  </si>
+  <si>
+    <t>Le trafic des sites internet est largement dû aux partages sociaux. C'est pour cela que deux principaux critères issus de Facebook seraient pris en compte par les algorithmes de pertinence des moteurs de recherche: les liens sociaux et la réputation de l'auteur. Insérer cet Open Graph va avoir un impact sur notre taux de clic.
+L’exemple classique étant: vous partagez un lien sur Facebook et la miniature d’image manque ou la mauvaise image apparaît. Plutôt énervant non? 
+L’Open Graph est la pour offrir une meilleure expérience utilisateur et pour optimiser les partages.</t>
+  </si>
+  <si>
+    <t>Créer un Open Graph aide à mieux comprendre le contenu d’une page web, il sert également au bon fonctionnement des réseaux sociaux, qui utilisent le protocole pour afficher le bon titre, la bonne description et la bonne image pour un partage.
+Il permet d’avoir un certain degré de contrôle sur l’information qui est partagée.</t>
+  </si>
+  <si>
+    <t>Créer un OpenGraph dans la balise head du fichier index.html et je vous conseil d'ajouter un bouton/raccourci J'aime (de Facebook en lien avec votre page).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sur la Page 2, le profil de l'entreprise (contact, adresse, horaires, …) n'est pas clairement visible et défini en plus du problème de mots-clés vu juste ci-dessus. Cela frêne le SEO local. 
+Il n'y a aucun retour de vos clients. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bichonner sa présence web en définissant un plan Google Business, un balisage de données structurées puis de répertorier et gérer les avis de clients pour avoir un meilleur taux de conversion.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Les données structurées sont du code que vous pouvez ajouter aux pages de votre site pour décrire votre contenu aux moteurs de recherche, de sorte qu'ils comprennent plus facilement ce qui se trouve sur vos pages. Les moteurs de recherche peuvent utiliser cette interprétation pour afficher votre contenu de manière utile (et accrocheuse !) dans les résultats de recherche. Cela peut vous aider à attirer le bon type de clients pour votre entreprise.</t>
+    </r>
+  </si>
+  <si>
+    <t>Réaliser une mise en page plus optimisée, ajouter un numéro de téléphone (standard) et demander à vos clients un retour sur votre prestation afin de créer une section d'avis / retour pour rassurer et donner envie à vos futurs clients (taux de conversion).
+Créer le balisage de données structurées pour donner les bonnes informations de contact au googlebots et à d'autres sites.</t>
+  </si>
+  <si>
+    <t>https://www.abondance.com/20200228-42120-infographie-6-points-essentiels-pour-reussir-son-seo-local.html
+https://smartkeyword.io/seo-outils-google-google-my-business/
+https://support.google.com/webmasters/answer/7451184?hl=fr
+Algorithme Pigeon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Pas de présence de fil d'Ariane.
+Si vous souhaitez rendre votre site attratif, vous allez développer un peu son contenu de manière pertinente et donc le fil d'Ariane va permettre de naviguer plus rapidement.
+</t>
     </r>
     <r>
       <rPr>
@@ -355,99 +420,215 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-Nous voyons sur l'index.html que les balises Hn de respectent pas la hiérarchie. Il est important d'utiliser ces balises pour fournir une information sémantique et non l'utiliser pour leur 'visuel'. C'est également un bon moyen d'introduire des mots-clés (expressions). Pour H1, il faut respecter l'ordre de grandeur (80 caractères max). Le H1 doit être légèrement différent de la balise title pour la longue traine.
+Le nom des URL peuvent aider vos utilisateurs à savoir où ils sont et permet un partage plus friendly mais Google va aussi rendre visible lors de la recherche. Une page2 n'est donc pas très pertinent.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>La présence d'un fil d'Ariane en utilisant les données structurées permettra également l'exploitation de ces informations par les googlebots.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Les URL avec des mots pertinents pour le contenu et la structure de votre site sont plus conviviales pour les visiteurs qui consultent votre site.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://support.google.com/webmasters/answer/7451184?hl=fr
 </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFC00000"/>
+        <color theme="7"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Le fait d'avoir une structure HTML5 correcte va permettre une meilleure lecture par les bots mais aussi pour les lecteurs d'écran.
+      <t>https://developers.google.com/search/docs/data-types/breadcrumb</t>
+    </r>
+  </si>
+  <si>
+    <t>sitemap image si non accessible pas écrit en dure &lt;img&gt;</t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/178636?vid=1-635753330792570943-3498756790084937771</t>
+  </si>
+  <si>
+    <t>https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/
+https://smartkeyword.io/seo-on-page-images-attribut-alt/</t>
+  </si>
+  <si>
+    <t>Renommer les images de manière à décrire ce qu'elles représentent, modifier/intégrer l'attribut alt (5/6 mots) pour qu'il soit personnalisé à l'image. 
+Redimensionner les images par rapport à son encart et les convertir dans un format optimisé.
+Na pas oublier le favicon</t>
+  </si>
+  <si>
+    <t>Les images doit être dimensionnées raisonnablement par rapport à son "encart d'accueil", optimisées et être dans un format adapté au web. Elles doivent comportées une description dans l'attribut 'alt' et qu'elle soit personnalisée (lu par les moteurs de recherche et les lecteurs d'écran),
+Elles doivent aussi être nommer correctement pour que les googlebots comprennent.</t>
+  </si>
+  <si>
+    <t>La taille des images, non optimisées et dans un format non adapté.
+-&gt; Budget crawl
+L'attribut alt est utilisé pour intégrer un tas de mots clés qui n'a rien à voir avec ce que l'image représente.
+-&gt; Google ne peut pas contextualiser, les lecteurs d'écran lisent des données non probantes, et lorsqu'il y a des ralentissements réseaux ou autre, les données affichées ne nous aident pas à comprendre.
+Les images ne sont pas coorectement nommé.
+-&gt; Google utilise le nom des images dans son visuel de recherche.</t>
+  </si>
+  <si>
+    <t>La page se charge en 1,8s. En 2017, Google révèle que plus de la moitié des mobinautes choisissent de fermer l’onglet d’une page qui ne se charge pas totalement au bout de 3 secondes. 
+En sachant que le site n'est pas très important en nombre d'articles, de photos, de fonctionnalités, ...
+Il est important pour vos utilisateurs, pour votre budget crawling et votre référencement d'optimiser la vitesse de chargement.
+Pour ce faire, en plus des images (vu précedemment), nous pouvons voir qu'un cache n'est défini, qu'il y a des redondances de code au sein d'une même déclaration CSS, que tous les fichiers ne sont pas minifier et que des ressources sont chargées trop tôt.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Utilisation des caches navigateurs, différé le chargement des fichiers secondaires et minifier le JS/CSS.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Attention aussi : 
+- aux ressources chargées trop tôt;
+- aux redondances d'un même code au sein d'une classe.</t>
+    </r>
+  </si>
+  <si>
+    <t>URL page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">https://www.webrankinfo.com/dossiers/referencement-mobile/speed-update
+https://www.webrankinfo.com/dossiers/webmastering/site-rapide
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.seo.fr/informations/vitesse
+https://openweb.eu.org/articles/le-fichier-htaccess
+https://openweb.eu.org/articles/performances_avancees_sites_internet</t>
+    </r>
+  </si>
+  <si>
+    <t>Réaliser un fichier htaccess : mise en cache, indiquer au serveur d'envoyer les fichiers compressés.</t>
+  </si>
+  <si>
+    <t>Utilisation sémantique des balises HTML5 (header, main, footer, nav, article, section, aside) construction du code en respectant une hiérarchie logique (h1 -&gt; h2 -&gt; h3 etc) et bien renseigner le title de la page. 
+N'avoir aucun code de style dans le fichier HTML.
+Il faut veiller à ne pas avoir des balises vident afin de ne pas perdre les lecteurs d'écran.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure HTML5 : il n'y a aucune balise html. Le fait d'avoir une structure HTML5 correcte va permettre une meilleure lecture pour les lecteurs d'écran et a pour but d’aider à la prise en compte de votre contenu pour les bots et d’en favoriser l’indexation et la position sur Google.
+Nous voyons sur l'index.html que les balises Hn de respectent pas la hiérarchie. Il est important d'utiliser ces balises pour fournir une information sémantique et non l'utiliser pour leur 'visuel'. C'est également un bon moyen d'introduire des mots-clés (expressions). Pour H1, il faut respecter l'ordre de grandeur (80 caractères max). Le H1 doit être légèrement différent de la balise title pour la longue traine.
 Des balises vides ont un aspect négatif sur les lecteurs d'écran. </t>
-    </r>
-  </si>
-  <si>
-    <t>ARIA ???</t>
-  </si>
-  <si>
-    <t>Références</t>
-  </si>
-  <si>
-    <t>https://fr.oncrawl.com/referencement/tout-ce-que-vous-devez-savoir-sur-lopen-graph/
-https://www.referenseo.com/guide-seo/open-graph/
-https://smartkeyword.io/seo-on-page-open-graph-twitter-card/</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>https://www.abondance.com/20200228-42120-infographie-6-points-essentiels-pour-reussir-son-seo-local.html</t>
-  </si>
-  <si>
-    <t>Bichonner sa présence web en définissant un plan Google Business puis de répertorier et gérer les avis de clients pour avoir un meilleur taux de conversion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sur la Page 2, le profil de l'entreprise (contact, adresse, horaires, …) n'est pas clairement visible et défini en plus du problème de mots-clés vu juste ci-dessus. Cela frêne le SEO local. 
+  </si>
+  <si>
+    <t>https://youtu.be/QWL864VlW7I
+John Mueller (webmaster trends analyst chez Google) dans un hangout avec les webmasters le 11/09/2015
+https://www.pixelcrea.com/blog/semantique-seo-page/
+https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/
+https://www.webrankinfo.com/dossiers/techniques/balises-h1-h2-h3</t>
+  </si>
+  <si>
+    <t>La langue doit être défini en respectant les normes déclaratives et ainsi permettre a lisibilité aux lecteurs d'écran</t>
+  </si>
+  <si>
+    <t>Cours OC :
+- Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques ;
+- Concevez un contenu web accessible.
+https://dequeuniversity.com/rules/axe/3.3/html-lang-valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cours OC Concevez un contenu web accessible
 </t>
   </si>
   <si>
-    <t>Réaliser une véritable campagne de netlinking.
-C'est-à-dire avoir des liens cohérents avec le contenu. Qu'il s'intègre dans l'information pour avoir une vrai plus-value et non une présence superficielle. 
-Liens : titre cohérent, follow les liens cohérents et nofollow les autres (voir les enlever), attribut des liens correctement déclarés.</t>
-  </si>
-  <si>
-    <t>Il faut donc garder ceux qui sont cohérents (et oui soignez vos sources !) et si possible ajouter du contexte/du sens. Envisagez de les enlever carrément du footer et de créer un article/du contenu de qualité en les intégrant pour obtenir du sens et une attraction pour l'utilisateur (situation du lien),
-Mettre des titres cohérents aux liens garder (anchor text)
-Définir si les bots doivent "lire/suivre/regarder" les liens.
-Nous oublions pas de bien déclarer correctement des attribut aux liens.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les liens en bas de page (dans le footer visuel) ne sont pas cohérents avec l'activité de l'agence et sont clairement des liens artificiels. On ne comprend pas pourquoi ils sont là. Et n'oublions pas que Google a fait et fait évoluer ses algorithmes pour comprendre le contexte. Des liens "parasites" peuvent faire pénaliser tout le site.  </t>
-  </si>
-  <si>
-    <t>https://analytics.moz.com/pro/keyword-explorer/
-https://support.google.com/webmasters/answer/79812?hl=fr
-Algorithme Google :Colibri et son amélioration, Rankbrain
-https://www.webrankinfo.com/dossiers/conseils/meta-description-seo
-https://www.webrankinfo.com/dossiers/debutants/balise-title
-https://www.webrankinfo.com/dossiers/conseils/balise-meta-description
-https://youtu.be/jK7IPbnmvVU
-https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
-  </si>
-  <si>
-    <t>Etude sur les mots-clés utilisés et la concurrence.
-Renseigner la balise Title et la Meta description en tilisant les bons mots-clés. Attention, il faut penser utilisateur et compréhension utilisateur ! En effet Google parfait ses algorithmes dans ce sens !
-Enlever la meta keyword qui n'a aucune plus-value car JAMAIS utilisé par les GoggleBots</t>
-  </si>
-  <si>
-    <t>Algorithme Pigeon de Google (2015)
-Cours OC Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques</t>
-  </si>
-  <si>
-    <t>Réaliser une mise en page et</t>
-  </si>
-  <si>
-    <t>Réaliser une multiplication des mots-clés de manière intempestives et cacher à l'utilisateur, que nous pouvons retrouver dans la page index.html et page2.html, est un procédé banni par Google et va même jusqu'à sanctionner en black-listant le site. 
-Index : class=keyword
-Page2 : h1 non visible</t>
-  </si>
-  <si>
-    <t>La langue définie est l'allemand pour un site entièrement écrit en français et les outils d'analyse détectent bien le français.
-Dans la page2, les messages informationnels concernant l'envoi/ou non doivent être dans la même langue.</t>
-  </si>
-  <si>
-    <t>Redéfinir correctement l'attribut lang et ne pas le mettre par défaut ("fr-fr").
-Ecrire en français pour votre auditoire lisant et écoutant (lecteurs d'écran) français.</t>
+    <t>Les liens n'ont pas assez d'espaces entre eux. Les infos contact sont beaucoup trop petites.
+Il y a des textes intégrés sous des images: manque de responsive en mobile, problème de lectures pour la technologie d'aide.</t>
+  </si>
+  <si>
+    <t>Enlever les images et les remplacer par du texte. Revoir la visibilité des liens.</t>
+  </si>
+  <si>
+    <t>https://www.codeur.com/blog/supprimer-code-css-inutile/</t>
+  </si>
+  <si>
+    <t>Les bots sont des vrais marathoniens ! 
+Pensons donc à ne pas surcharger leur parcours avec des fichiers qui ne sont pas utilisés ni utile au fonctionnement du site.
+Gain de vitesse, de ressources et donc vive le budget crawling !</t>
+  </si>
+  <si>
+    <t>Le site a été codé avec bootstrap. Ce framework est livré avec une bibilothèque complète. Mais nous n'utilisons pas la globalité de la bibliothèque. Notre navigateur les télécharge quand même : perte de vitesse et du budget crawling.</t>
+  </si>
+  <si>
+    <t>Supprimer le code qui n'est pas utilisé (82,88% du code css n'est pas utilisé).</t>
+  </si>
+  <si>
+    <t>https://stephaniewalter.design/fr/blog/accessibilite-et-couleurs-outils-et-ressources-pour-concevoir-des-produits-accessible/
+http://www.handi-pratique.com/contraste-couleurs-accessibilite-web</t>
+  </si>
+  <si>
+    <t>Couleurs et Contrastes : le Ying et le Yang de l'accessibilité visuelle de base.</t>
+  </si>
+  <si>
+    <t>Pensons que certaines personnes ont un handicap visuel (daltonien / malvoyant). Pour cela, le choix des couleurs est important pour assurer une bonne visibilité du contenu.</t>
+  </si>
+  <si>
+    <t>Le site ne passe pas avec succès les normes d'accessibilité défini.</t>
+  </si>
+  <si>
+    <t>Revoir les défauts de contraste et choisir les couleurs de remplacement pour assurer un niveau de contraste optimal.</t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/6062596?hl=fr
+https://www.seoh.fr/seo-technique/le-guide-ultime-du-fichier-robots-txt.html</t>
+  </si>
+  <si>
+    <t>Définir une balise noscript.
+La &lt;noscript&gt;balise définit un autre contenu à afficher pour les utilisateurs qui ont des scripts désactivés dans leur navigateur ou qui ont un navigateur qui ne prend pas en charge les scripts.</t>
+  </si>
+  <si>
+    <t>Dans le cas où les scripts ne chargeraient pas, il est fortement conseillé d'afficher un message pour l'utilisateur avec la balise noscript.
+Sur le site aucune balise noscript n'est défini.</t>
+  </si>
+  <si>
+    <t>Mettre en place la balise noscript</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/noscript
+https://www.w3schools.com/tags/tag_noscript.asp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -458,16 +639,19 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -520,20 +704,44 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,6 +796,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -609,7 +823,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,9 +868,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -668,7 +879,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -680,9 +891,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -691,6 +899,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -908,11 +1146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -940,8 +1178,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>87</v>
+      <c r="F1" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -964,24 +1202,24 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="36" t="s">
+    <row r="2" spans="1:26" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>98</v>
+      <c r="B2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1005,23 +1243,23 @@
       <c r="Z2" s="12"/>
     </row>
     <row r="3" spans="1:26" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>80</v>
+      <c r="B3" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1045,23 +1283,23 @@
       <c r="Z3" s="12"/>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>96</v>
+      <c r="B4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -1084,24 +1322,24 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
     </row>
-    <row r="5" spans="1:26" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:26" s="13" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D5" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="40" t="s">
         <v>91</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -1124,21 +1362,23 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
     </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+    <row r="6" spans="1:26" s="13" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="40" t="s">
+        <v>94</v>
+      </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -1160,24 +1400,24 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>46</v>
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1200,22 +1440,24 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>34</v>
+    <row r="8" spans="1:26" s="13" customFormat="1" ht="270" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>79</v>
+        <v>49</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1238,19 +1480,25 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>49</v>
+    <row r="9" spans="1:26" s="13" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="42" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="C9" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>104</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -1272,19 +1520,25 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>34</v>
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+        <v>59</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>111</v>
+      </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -1307,16 +1561,24 @@
       <c r="Z10" s="12"/>
     </row>
     <row r="11" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>49</v>
+      <c r="A11" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>114</v>
+      </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -1339,19 +1601,23 @@
       <c r="Z11" s="12"/>
     </row>
     <row r="12" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="31" t="s">
-        <v>88</v>
+      <c r="A12" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>118</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -1374,19 +1640,25 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:26" s="13" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+        <v>56</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>74</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -1409,18 +1681,20 @@
       <c r="Z13" s="12"/>
     </row>
     <row r="14" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>49</v>
+      <c r="A14" s="45" t="s">
+        <v>34</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -1442,24 +1716,24 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
-        <v>34</v>
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>76</v>
+        <v>55</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>127</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1482,270 +1756,317 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" spans="1:26" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="16" spans="1:26" s="13" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+    </row>
+    <row r="17" spans="1:26" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
+      <c r="Z17" s="21"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="C19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F19" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="4" t="s">
+      <c r="G19" s="43"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="14" t="s">
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="5" t="s">
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>41</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>16</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="15" t="s">
-        <v>19</v>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="16" t="s">
-        <v>20</v>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="15" t="s">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D29" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="15" t="s">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D30" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="15" t="s">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D31" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="15" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D33" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="15"/>
-      <c r="D33" s="18" t="s">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="15"/>
+      <c r="D34" s="18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="15" t="s">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="26" t="s">
-        <v>71</v>
+      <c r="A42" s="25" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="10" t="s">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C50" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2698,15 +3019,17 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F18:G23"/>
+    <mergeCell ref="F19:G24"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C49" r:id="rId1" xr:uid="{AB5B6FFC-1D25-4AAE-B717-307BDF0802B7}"/>
-    <hyperlink ref="C50" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
+    <hyperlink ref="C50" r:id="rId1" xr:uid="{AB5B6FFC-1D25-4AAE-B717-307BDF0802B7}"/>
+    <hyperlink ref="C51" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
+    <hyperlink ref="A57" r:id="rId3" xr:uid="{D5DF4612-2C0B-4E4B-8073-2ADEFE0970DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Telechargement 1er fichier Changement : enlever les keywords des alt, les balises non essentiel + integration header, section, footer, enlever les liens inutile dans le footer
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F7A8AE-38C5-449A-9C1F-2E36A13304B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570FDF27-EECB-4416-9EC1-61DFDD81F97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$16</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -803,7 +806,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -818,6 +821,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -825,9 +843,6 @@
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -841,9 +856,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -873,61 +885,67 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1146,11 +1164,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD15"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1163,671 +1184,671 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-    </row>
-    <row r="3" spans="1:26" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+    </row>
+    <row r="3" spans="1:26" s="11" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-    </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" ht="255" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+    </row>
+    <row r="4" spans="1:26" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" s="13" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+    </row>
+    <row r="5" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-    </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+    </row>
+    <row r="6" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="40" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-    </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+    </row>
+    <row r="7" spans="1:26" s="11" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
-    </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" ht="270" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+    </row>
+    <row r="8" spans="1:26" s="11" customFormat="1" ht="270" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-    </row>
-    <row r="9" spans="1:26" s="13" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+    </row>
+    <row r="9" spans="1:26" s="11" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
-    </row>
-    <row r="10" spans="1:26" s="13" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+    </row>
+    <row r="10" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-    </row>
-    <row r="11" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+    </row>
+    <row r="11" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="40" t="s">
         <v>117</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-    </row>
-    <row r="12" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+    </row>
+    <row r="12" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="40" t="s">
         <v>122</v>
       </c>
       <c r="F12" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
-    </row>
-    <row r="13" spans="1:26" s="13" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+    </row>
+    <row r="13" spans="1:26" s="11" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-    </row>
-    <row r="14" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+    </row>
+    <row r="14" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-    </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+    </row>
+    <row r="15" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="40" t="s">
         <v>126</v>
       </c>
       <c r="F15" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-    </row>
-    <row r="16" spans="1:26" s="13" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+    </row>
+    <row r="16" spans="1:26" s="11" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-    </row>
-    <row r="17" spans="1:26" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+    </row>
+    <row r="17" spans="1:26" s="20" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
@@ -1841,113 +1862,113 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="43"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1955,74 +1976,74 @@
       <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="15"/>
-      <c r="D34" s="18" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="23" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="22" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2031,18 +2052,18 @@
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="24" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2051,12 +2072,12 @@
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="24" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3029,7 +3050,7 @@
     <hyperlink ref="C51" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
     <hyperlink ref="A57" r:id="rId3" xr:uid="{D5DF4612-2C0B-4E4B-8073-2ADEFE0970DC}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId4"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
format image et alléger
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570FDF27-EECB-4416-9EC1-61DFDD81F97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1EE8C7-EE37-489E-9D36-1651503181AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -885,9 +885,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -947,6 +944,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1170,8 +1170,8 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1184,22 +1184,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1"/>
@@ -1224,22 +1224,22 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>110</v>
       </c>
       <c r="G2" s="10"/>
@@ -1264,22 +1264,22 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="1:26" s="11" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>69</v>
       </c>
       <c r="G3" s="10"/>
@@ -1304,22 +1304,22 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="1:26" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="10"/>
@@ -1344,22 +1344,22 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="35" t="s">
         <v>91</v>
       </c>
       <c r="G5" s="10"/>
@@ -1384,20 +1384,20 @@
       <c r="Z5" s="10"/>
     </row>
     <row r="6" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="36" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="35" t="s">
         <v>94</v>
       </c>
       <c r="G6" s="10"/>
@@ -1422,22 +1422,22 @@
       <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" s="11" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="40" t="s">
         <v>97</v>
       </c>
       <c r="G7" s="10"/>
@@ -1462,22 +1462,22 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" s="11" customFormat="1" ht="270" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="41" t="s">
         <v>108</v>
       </c>
       <c r="G8" s="10"/>
@@ -1502,22 +1502,22 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" s="11" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="39" t="s">
         <v>104</v>
       </c>
       <c r="G9" s="10"/>
@@ -1542,22 +1542,22 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="39" t="s">
         <v>111</v>
       </c>
       <c r="G10" s="10"/>
@@ -1582,22 +1582,22 @@
       <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="43" t="s">
         <v>114</v>
       </c>
       <c r="G11" s="10"/>
@@ -1622,22 +1622,22 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="43" t="s">
         <v>118</v>
       </c>
       <c r="G12" s="10"/>
@@ -1662,22 +1662,22 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="1:26" s="11" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="40" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="10"/>
@@ -1702,18 +1702,18 @@
       <c r="Z13" s="10"/>
     </row>
     <row r="14" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="44" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="43" t="s">
         <v>123</v>
       </c>
       <c r="G14" s="10"/>
@@ -1738,22 +1738,22 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="43" t="s">
         <v>127</v>
       </c>
       <c r="G15" s="10"/>
@@ -1778,22 +1778,22 @@
       <c r="Z15" s="10"/>
     </row>
     <row r="16" spans="1:26" s="11" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="38" t="s">
         <v>67</v>
       </c>
       <c r="G16" s="10"/>
@@ -1868,18 +1868,18 @@
       <c r="E19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="25"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="3" t="s">
@@ -1888,8 +1888,8 @@
       <c r="D22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="12" t="s">
@@ -1898,8 +1898,8 @@
       <c r="D23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
@@ -1911,8 +1911,8 @@
       <c r="D24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="4" t="s">

</xml_diff>

<commit_message>
Image alleger + .htaccess mise en cache img
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1EE8C7-EE37-489E-9D36-1651503181AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21EF2AC-66CB-4F58-BDB9-678C6F7045D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1170,8 +1170,8 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Correction fautes de frappe + tabl a jour + reco
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880EDF90-D2A7-4BD2-9E02-17FF702A5ADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF9DBBF-7E99-4BBE-B9B8-44FFB532F916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$16</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="129">
   <si>
     <t>Categorie</t>
   </si>
@@ -346,22 +347,6 @@
   </si>
   <si>
     <t>Supprimer ce morceau de code et se concentrer sur les bonnes pratique White Hat pour obtenir un SEO viable et plus stable. Vous éviterez ainsi de vous faire blacklister par les Googlebots,</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Réaliser une multiplication des mots-clés de manière intempestives et cacher à l'utilisateur, que nous pouvons retrouver dans la page index.html et page2.html, est un procédé banni par Google et va même jusqu'à sanctionner en black-listant le site. 
-Index : class=keyword
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Page2 : h1 non visible</t>
-    </r>
   </si>
   <si>
     <t>Le trafic des sites internet est largement dû aux partages sociaux. C'est pour cela que deux principaux critères issus de Facebook seraient pris en compte par les algorithmes de pertinence des moteurs de recherche: les liens sociaux et la réputation de l'auteur. Insérer cet Open Graph va avoir un impact sur notre taux de clic.
@@ -403,63 +388,6 @@
 https://smartkeyword.io/seo-outils-google-google-my-business/
 https://support.google.com/webmasters/answer/7451184?hl=fr
 Algorithme Pigeon</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Pas de présence de fil d'Ariane.
-Si vous souhaitez rendre votre site attratif, vous allez développer un peu son contenu de manière pertinente et donc le fil d'Ariane va permettre de naviguer plus rapidement.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Le nom des URL peuvent aider vos utilisateurs à savoir où ils sont et permet un partage plus friendly mais Google va aussi rendre visible lors de la recherche. Une page2 n'est donc pas très pertinent.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>La présence d'un fil d'Ariane en utilisant les données structurées permettra également l'exploitation de ces informations par les googlebots.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Les URL avec des mots pertinents pour le contenu et la structure de votre site sont plus conviviales pour les visiteurs qui consultent votre site.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">https://support.google.com/webmasters/answer/7451184?hl=fr
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://developers.google.com/search/docs/data-types/breadcrumb</t>
-    </r>
   </si>
   <si>
     <t>sitemap image si non accessible pas écrit en dure &lt;img&gt;</t>
@@ -513,6 +441,102 @@
   </si>
   <si>
     <t>URL page</t>
+  </si>
+  <si>
+    <t>Utilisation sémantique des balises HTML5 (header, main, footer, nav, article, section, aside) construction du code en respectant une hiérarchie logique (h1 -&gt; h2 -&gt; h3 etc) et bien renseigner le title de la page. 
+N'avoir aucun code de style dans le fichier HTML.
+Il faut veiller à ne pas avoir des balises vident afin de ne pas perdre les lecteurs d'écran.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure HTML5 : il n'y a aucune balise html. Le fait d'avoir une structure HTML5 correcte va permettre une meilleure lecture pour les lecteurs d'écran et a pour but d’aider à la prise en compte de votre contenu pour les bots et d’en favoriser l’indexation et la position sur Google.
+Nous voyons sur l'index.html que les balises Hn de respectent pas la hiérarchie. Il est important d'utiliser ces balises pour fournir une information sémantique et non l'utiliser pour leur 'visuel'. C'est également un bon moyen d'introduire des mots-clés (expressions). Pour H1, il faut respecter l'ordre de grandeur (80 caractères max). Le H1 doit être légèrement différent de la balise title pour la longue traine.
+Des balises vides ont un aspect négatif sur les lecteurs d'écran. </t>
+  </si>
+  <si>
+    <t>https://youtu.be/QWL864VlW7I
+John Mueller (webmaster trends analyst chez Google) dans un hangout avec les webmasters le 11/09/2015
+https://www.pixelcrea.com/blog/semantique-seo-page/
+https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/
+https://www.webrankinfo.com/dossiers/techniques/balises-h1-h2-h3</t>
+  </si>
+  <si>
+    <t>La langue doit être défini en respectant les normes déclaratives et ainsi permettre a lisibilité aux lecteurs d'écran</t>
+  </si>
+  <si>
+    <t>Cours OC :
+- Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques ;
+- Concevez un contenu web accessible.
+https://dequeuniversity.com/rules/axe/3.3/html-lang-valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cours OC Concevez un contenu web accessible
+</t>
+  </si>
+  <si>
+    <t>Les liens n'ont pas assez d'espaces entre eux. Les infos contact sont beaucoup trop petites.
+Il y a des textes intégrés sous des images: manque de responsive en mobile, problème de lectures pour la technologie d'aide.</t>
+  </si>
+  <si>
+    <t>Enlever les images et les remplacer par du texte. Revoir la visibilité des liens.</t>
+  </si>
+  <si>
+    <t>https://www.codeur.com/blog/supprimer-code-css-inutile/</t>
+  </si>
+  <si>
+    <t>Les bots sont des vrais marathoniens ! 
+Pensons donc à ne pas surcharger leur parcours avec des fichiers qui ne sont pas utilisés ni utile au fonctionnement du site.
+Gain de vitesse, de ressources et donc vive le budget crawling !</t>
+  </si>
+  <si>
+    <t>Le site a été codé avec bootstrap. Ce framework est livré avec une bibilothèque complète. Mais nous n'utilisons pas la globalité de la bibliothèque. Notre navigateur les télécharge quand même : perte de vitesse et du budget crawling.</t>
+  </si>
+  <si>
+    <t>Supprimer le code qui n'est pas utilisé (82,88% du code css n'est pas utilisé).</t>
+  </si>
+  <si>
+    <t>https://stephaniewalter.design/fr/blog/accessibilite-et-couleurs-outils-et-ressources-pour-concevoir-des-produits-accessible/
+http://www.handi-pratique.com/contraste-couleurs-accessibilite-web</t>
+  </si>
+  <si>
+    <t>Couleurs et Contrastes : le Ying et le Yang de l'accessibilité visuelle de base.</t>
+  </si>
+  <si>
+    <t>Pensons que certaines personnes ont un handicap visuel (daltonien / malvoyant). Pour cela, le choix des couleurs est important pour assurer une bonne visibilité du contenu.</t>
+  </si>
+  <si>
+    <t>Le site ne passe pas avec succès les normes d'accessibilité défini.</t>
+  </si>
+  <si>
+    <t>Revoir les défauts de contraste et choisir les couleurs de remplacement pour assurer un niveau de contraste optimal.</t>
+  </si>
+  <si>
+    <t>https://support.google.com/webmasters/answer/6062596?hl=fr
+https://www.seoh.fr/seo-technique/le-guide-ultime-du-fichier-robots-txt.html</t>
+  </si>
+  <si>
+    <t>Définir une balise noscript.
+La &lt;noscript&gt;balise définit un autre contenu à afficher pour les utilisateurs qui ont des scripts désactivés dans leur navigateur ou qui ont un navigateur qui ne prend pas en charge les scripts.</t>
+  </si>
+  <si>
+    <t>Dans le cas où les scripts ne chargeraient pas, il est fortement conseillé d'afficher un message pour l'utilisateur avec la balise noscript.
+Sur le site aucune balise noscript n'est défini.</t>
+  </si>
+  <si>
+    <t>Mettre en place la balise noscript</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/noscript
+https://www.w3schools.com/tags/tag_noscript.asp</t>
+  </si>
+  <si>
+    <t>Les URL avec des mots pertinents pour le contenu et la structure de votre site sont plus conviviales pour les visiteurs qui consultent votre site.</t>
+  </si>
+  <si>
+    <t>Le nom des URL peuvent aider vos utilisateurs à savoir où ils sont et permet un partage plus friendly mais Google va aussi rendre visible lors de la recherche. Une page2 n'est donc pas très pertinent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://support.google.com/webmasters/answer/7451184?hl=fr
+</t>
   </si>
   <si>
     <r>
@@ -534,104 +558,38 @@
       </rPr>
       <t>https://www.seo.fr/informations/vitesse
 https://openweb.eu.org/articles/le-fichier-htaccess
-https://openweb.eu.org/articles/performances_avancees_sites_internet</t>
+https://openweb.eu.org/articles/performances_avancees_sites_internet
+https://web.dev/defer-non-critical-css/</t>
     </r>
   </si>
   <si>
-    <t>Réaliser un fichier htaccess : mise en cache, indiquer au serveur d'envoyer les fichiers compressés.</t>
-  </si>
-  <si>
-    <t>Utilisation sémantique des balises HTML5 (header, main, footer, nav, article, section, aside) construction du code en respectant une hiérarchie logique (h1 -&gt; h2 -&gt; h3 etc) et bien renseigner le title de la page. 
-N'avoir aucun code de style dans le fichier HTML.
-Il faut veiller à ne pas avoir des balises vident afin de ne pas perdre les lecteurs d'écran.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure HTML5 : il n'y a aucune balise html. Le fait d'avoir une structure HTML5 correcte va permettre une meilleure lecture pour les lecteurs d'écran et a pour but d’aider à la prise en compte de votre contenu pour les bots et d’en favoriser l’indexation et la position sur Google.
-Nous voyons sur l'index.html que les balises Hn de respectent pas la hiérarchie. Il est important d'utiliser ces balises pour fournir une information sémantique et non l'utiliser pour leur 'visuel'. C'est également un bon moyen d'introduire des mots-clés (expressions). Pour H1, il faut respecter l'ordre de grandeur (80 caractères max). Le H1 doit être légèrement différent de la balise title pour la longue traine.
-Des balises vides ont un aspect négatif sur les lecteurs d'écran. </t>
-  </si>
-  <si>
-    <t>https://youtu.be/QWL864VlW7I
-John Mueller (webmaster trends analyst chez Google) dans un hangout avec les webmasters le 11/09/2015
-https://www.pixelcrea.com/blog/semantique-seo-page/
-https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/
-https://www.webrankinfo.com/dossiers/techniques/balises-h1-h2-h3</t>
-  </si>
-  <si>
-    <t>La langue doit être défini en respectant les normes déclaratives et ainsi permettre a lisibilité aux lecteurs d'écran</t>
-  </si>
-  <si>
-    <t>Cours OC :
-- Optimisez le référencement de votre site (SEO) en améliorant ses performances techniques ;
-- Concevez un contenu web accessible.
-https://dequeuniversity.com/rules/axe/3.3/html-lang-valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cours OC Concevez un contenu web accessible
+    <t>Réaliser un fichier htaccess : mise en cache, indiquer au serveur d'envoyer les fichiers compressés et paramétré les chargements différés des scripts et styles,</t>
+  </si>
+  <si>
+    <t>Renommer la page2.html.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Réaliser une multiplication des mots-clés de manière intempestives et cacher à l'utilisateur, que nous pouvons retrouver dans la page index.html et page2.html, est un procédé banni par Google et va même jusqu'à sanctionner en black-listant le site. 
+Index : class=keyword
 </t>
-  </si>
-  <si>
-    <t>Les liens n'ont pas assez d'espaces entre eux. Les infos contact sont beaucoup trop petites.
-Il y a des textes intégrés sous des images: manque de responsive en mobile, problème de lectures pour la technologie d'aide.</t>
-  </si>
-  <si>
-    <t>Enlever les images et les remplacer par du texte. Revoir la visibilité des liens.</t>
-  </si>
-  <si>
-    <t>https://www.codeur.com/blog/supprimer-code-css-inutile/</t>
-  </si>
-  <si>
-    <t>Les bots sont des vrais marathoniens ! 
-Pensons donc à ne pas surcharger leur parcours avec des fichiers qui ne sont pas utilisés ni utile au fonctionnement du site.
-Gain de vitesse, de ressources et donc vive le budget crawling !</t>
-  </si>
-  <si>
-    <t>Le site a été codé avec bootstrap. Ce framework est livré avec une bibilothèque complète. Mais nous n'utilisons pas la globalité de la bibliothèque. Notre navigateur les télécharge quand même : perte de vitesse et du budget crawling.</t>
-  </si>
-  <si>
-    <t>Supprimer le code qui n'est pas utilisé (82,88% du code css n'est pas utilisé).</t>
-  </si>
-  <si>
-    <t>https://stephaniewalter.design/fr/blog/accessibilite-et-couleurs-outils-et-ressources-pour-concevoir-des-produits-accessible/
-http://www.handi-pratique.com/contraste-couleurs-accessibilite-web</t>
-  </si>
-  <si>
-    <t>Couleurs et Contrastes : le Ying et le Yang de l'accessibilité visuelle de base.</t>
-  </si>
-  <si>
-    <t>Pensons que certaines personnes ont un handicap visuel (daltonien / malvoyant). Pour cela, le choix des couleurs est important pour assurer une bonne visibilité du contenu.</t>
-  </si>
-  <si>
-    <t>Le site ne passe pas avec succès les normes d'accessibilité défini.</t>
-  </si>
-  <si>
-    <t>Revoir les défauts de contraste et choisir les couleurs de remplacement pour assurer un niveau de contraste optimal.</t>
-  </si>
-  <si>
-    <t>https://support.google.com/webmasters/answer/6062596?hl=fr
-https://www.seoh.fr/seo-technique/le-guide-ultime-du-fichier-robots-txt.html</t>
-  </si>
-  <si>
-    <t>Définir une balise noscript.
-La &lt;noscript&gt;balise définit un autre contenu à afficher pour les utilisateurs qui ont des scripts désactivés dans leur navigateur ou qui ont un navigateur qui ne prend pas en charge les scripts.</t>
-  </si>
-  <si>
-    <t>Dans le cas où les scripts ne chargeraient pas, il est fortement conseillé d'afficher un message pour l'utilisateur avec la balise noscript.
-Sur le site aucune balise noscript n'est défini.</t>
-  </si>
-  <si>
-    <t>Mettre en place la balise noscript</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/fr/docs/Web/HTML/Element/noscript
-https://www.w3schools.com/tags/tag_noscript.asp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Page2 : h1 non visible</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -715,12 +673,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="7"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -744,7 +696,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,25 +741,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -891,77 +831,44 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1185,36 +1092,37 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="5" width="45.5546875" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="51.21875" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" customWidth="1"/>
+    <col min="5" max="6" width="51.21875" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="32" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1"/>
@@ -1238,24 +1146,24 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="30" t="s">
-        <v>110</v>
+      <c r="F2" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -1278,23 +1186,23 @@
       <c r="Y2" s="10"/>
       <c r="Z2" s="10"/>
     </row>
-    <row r="3" spans="1:26" s="11" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="25" t="s">
         <v>69</v>
       </c>
       <c r="G3" s="10"/>
@@ -1318,23 +1226,23 @@
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
     </row>
-    <row r="4" spans="1:26" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:26" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="33" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="10"/>
@@ -1358,24 +1266,24 @@
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
     </row>
-    <row r="5" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:26" s="11" customFormat="1" ht="136.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>90</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>91</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -1398,22 +1306,24 @@
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="1:26" s="11" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:26" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="35" t="s">
-        <v>94</v>
+      <c r="B6" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -1436,24 +1346,24 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="1:26" s="11" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:26" s="11" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>97</v>
+      <c r="C7" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1476,24 +1386,24 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
     </row>
-    <row r="8" spans="1:26" s="11" customFormat="1" ht="270" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:26" s="11" customFormat="1" ht="225.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="39" t="s">
+      <c r="C8" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="41" t="s">
-        <v>108</v>
+      <c r="F8" s="33" t="s">
+        <v>102</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1516,24 +1426,24 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" s="11" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+    <row r="9" spans="1:26" s="11" customFormat="1" ht="165" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>104</v>
+      <c r="C9" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>125</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1557,23 +1467,23 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>111</v>
+      <c r="D10" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1596,24 +1506,24 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
     </row>
-    <row r="11" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48" t="s">
+    <row r="11" spans="1:26" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>114</v>
+      <c r="C11" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1636,24 +1546,24 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
     </row>
-    <row r="12" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>118</v>
+      <c r="B12" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1676,23 +1586,23 @@
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
     </row>
-    <row r="13" spans="1:26" s="11" customFormat="1" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:26" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="33" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="10"/>
@@ -1716,20 +1626,20 @@
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
     </row>
-    <row r="14" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+    <row r="14" spans="1:26" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="43" t="s">
-        <v>123</v>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="36" t="s">
+        <v>117</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1752,24 +1662,24 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
     </row>
-    <row r="15" spans="1:26" s="11" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:26" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="43" t="s">
-        <v>127</v>
+      <c r="C15" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>121</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1792,23 +1702,23 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
     </row>
-    <row r="16" spans="1:26" s="11" customFormat="1" ht="216.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:26" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="25" t="s">
         <v>67</v>
       </c>
       <c r="G16" s="10"/>
@@ -1832,277 +1742,12 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
     </row>
-    <row r="17" spans="1:26" s="20" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="45"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-    </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="13"/>
-      <c r="D34" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3057,16 +2702,302 @@
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{13A86D72-B05B-4CB7-98FB-240F186ECA86}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{7FB24903-87A1-4B7B-9D94-3A47EFCC17EF}"/>
+  </hyperlinks>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="51" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial,Gras"&amp;20&amp;K7030A0Fichier d'analyse SEO</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C0137B-5132-46E3-9B1E-EBD3898AB9F3}">
+  <dimension ref="A1:Z42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:26" s="20" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="13"/>
+      <c r="D18" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F19:G24"/>
+    <mergeCell ref="F3:G8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C50" r:id="rId1" xr:uid="{AB5B6FFC-1D25-4AAE-B717-307BDF0802B7}"/>
-    <hyperlink ref="C51" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
-    <hyperlink ref="A57" r:id="rId3" xr:uid="{D5DF4612-2C0B-4E4B-8073-2ADEFE0970DC}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{13A86D72-B05B-4CB7-98FB-240F186ECA86}"/>
+    <hyperlink ref="C34" r:id="rId1" xr:uid="{AB5B6FFC-1D25-4AAE-B717-307BDF0802B7}"/>
+    <hyperlink ref="C35" r:id="rId2" xr:uid="{861BB0BD-48FF-4801-AF5B-E25C2114869B}"/>
+    <hyperlink ref="A41" r:id="rId3" xr:uid="{D5DF4612-2C0B-4E4B-8073-2ADEFE0970DC}"/>
   </hyperlinks>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="landscape" r:id="rId5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifications annexe et index
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF9DBBF-7E99-4BBE-B9B8-44FFB532F916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A1140D-3D23-4774-9285-A684F1D25E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -837,9 +837,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -869,6 +866,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1092,8 +1092,8 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1102,27 +1102,28 @@
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="51.21875" customWidth="1"/>
     <col min="4" max="4" width="53.44140625" customWidth="1"/>
-    <col min="5" max="6" width="51.21875" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
+    <col min="6" max="6" width="51.21875" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1"/>
@@ -1147,7 +1148,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -1186,8 +1187,8 @@
       <c r="Y2" s="10"/>
       <c r="Z2" s="10"/>
     </row>
-    <row r="3" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -1227,7 +1228,7 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="1:26" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -1236,13 +1237,13 @@
       <c r="C4" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>70</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="10"/>
@@ -1267,7 +1268,7 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" s="11" customFormat="1" ht="136.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -1282,7 +1283,7 @@
       <c r="E5" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="32" t="s">
         <v>90</v>
       </c>
       <c r="G5" s="10"/>
@@ -1322,7 +1323,7 @@
       <c r="E6" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="33" t="s">
         <v>124</v>
       </c>
       <c r="G6" s="10"/>
@@ -1346,8 +1347,8 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="1:26" s="11" customFormat="1" ht="180" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:26" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1362,7 +1363,7 @@
       <c r="E7" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="32" t="s">
         <v>93</v>
       </c>
       <c r="G7" s="10"/>
@@ -1387,7 +1388,7 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" s="11" customFormat="1" ht="225.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -1402,7 +1403,7 @@
       <c r="E8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="32" t="s">
         <v>102</v>
       </c>
       <c r="G8" s="10"/>
@@ -1427,7 +1428,7 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" s="11" customFormat="1" ht="165" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -1467,7 +1468,7 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1522,7 +1523,7 @@
       <c r="E11" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="33" t="s">
         <v>108</v>
       </c>
       <c r="G11" s="10"/>
@@ -1547,7 +1548,7 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12" spans="1:26" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="26" t="s">
@@ -1562,7 +1563,7 @@
       <c r="E12" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="35" t="s">
         <v>112</v>
       </c>
       <c r="G12" s="10"/>
@@ -1587,7 +1588,7 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="1:26" s="11" customFormat="1" ht="150" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -1602,7 +1603,7 @@
       <c r="E13" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="32" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="10"/>
@@ -1638,7 +1639,7 @@
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="35" t="s">
         <v>117</v>
       </c>
       <c r="G14" s="10"/>
@@ -1663,7 +1664,7 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -1678,7 +1679,7 @@
       <c r="E15" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="35" t="s">
         <v>121</v>
       </c>
       <c r="G15" s="10"/>
@@ -1703,7 +1704,7 @@
       <c r="Z15" s="10"/>
     </row>
     <row r="16" spans="1:26" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -2718,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C0137B-5132-46E3-9B1E-EBD3898AB9F3}">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD42"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2775,18 +2776,18 @@
       <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -2795,8 +2796,8 @@
       <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
@@ -2805,8 +2806,8 @@
       <c r="D7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -2818,8 +2819,8 @@
       <c r="D8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">

</xml_diff>

<commit_message>
Modif annexe + donnees structurees
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128CC6E5-CD18-4EDA-8491-307C1BE19AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C913C7F-D8C3-4C85-834C-C55A0013C643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,7 +678,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,12 +727,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -769,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -817,9 +811,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,8 +1062,8 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1087,22 +1078,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>73</v>
       </c>
       <c r="G1" s="1"/>
@@ -1222,7 +1213,7 @@
       <c r="E4" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="10"/>
@@ -1247,7 +1238,7 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" s="11" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -1262,7 +1253,7 @@
       <c r="E5" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G5" s="10"/>
@@ -1302,7 +1293,7 @@
       <c r="E6" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>123</v>
       </c>
       <c r="G6" s="10"/>
@@ -1342,7 +1333,7 @@
       <c r="E7" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="30" t="s">
         <v>92</v>
       </c>
       <c r="G7" s="10"/>
@@ -1382,7 +1373,7 @@
       <c r="E8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>101</v>
       </c>
       <c r="G8" s="10"/>
@@ -1407,7 +1398,7 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" s="11" customFormat="1" ht="165" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -1502,7 +1493,7 @@
       <c r="E11" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="31" t="s">
         <v>107</v>
       </c>
       <c r="G11" s="10"/>
@@ -1542,7 +1533,7 @@
       <c r="E12" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="33" t="s">
         <v>111</v>
       </c>
       <c r="G12" s="10"/>
@@ -1582,7 +1573,7 @@
       <c r="E13" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="30" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="10"/>
@@ -1618,7 +1609,7 @@
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="33" t="s">
         <v>116</v>
       </c>
       <c r="G14" s="10"/>
@@ -1643,7 +1634,7 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -1658,7 +1649,7 @@
       <c r="E15" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="33" t="s">
         <v>120</v>
       </c>
       <c r="G15" s="10"/>
@@ -2755,18 +2746,18 @@
       <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
@@ -2775,8 +2766,8 @@
       <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
@@ -2785,8 +2776,8 @@
       <c r="D7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -2798,8 +2789,8 @@
       <c r="D8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">

</xml_diff>

<commit_message>
Revu du differ css
</commit_message>
<xml_diff>
--- a/annexes/Analyse_accessibilite_seo.xlsx
+++ b/annexes/Analyse_accessibilite_seo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\P4\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C82D79-C1D0-487A-81CE-D6C326838220}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D19807F-47E3-4D4C-91E1-50A7E1BB37DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1044,9 +1044,9 @@
   </sheetPr>
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1055,7 +1055,7 @@
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="A15" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="26" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="26" t="s">

</xml_diff>